<commit_message>
Fixed some stuff and made it run on mac.
Next is making cyclical excecution and plotting!
Cya !
</commit_message>
<xml_diff>
--- a/ExcelFolder/Test.xlsx
+++ b/ExcelFolder/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamfl\Desktop\Skripte\PapaFBA\ExcelTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/floriangrun/Desktop/repos/AmazonTracker/ExcelFolder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B8B6BF-C413-4920-9AF2-53863B459EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E86436-A4CB-CE4F-89A9-41E58093CB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -83,8 +83,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -365,25 +365,25 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14:I14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="63" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>